<commit_message>
extend ME program RWTH, TUBerlin, TUBraunschweig
</commit_message>
<xml_diff>
--- a/database/MechanicalEngineering/ME_Course_database.xlsx
+++ b/database/MechanicalEngineering/ME_Course_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\MechanicalEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476BB392-DCC6-432F-8F19-49DC470F87BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C8CECE-C424-45BE-88F6-DF4839A3B677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
     <sheet name="All_ME_Courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>普通物理學(一)</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>能源系統</t>
+  </si>
+  <si>
+    <t>製造學</t>
   </si>
 </sst>
 </file>
@@ -763,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
-  <dimension ref="A1:W424"/>
+  <dimension ref="A1:W425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1983,7 +1986,7 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="12" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
@@ -2007,7 +2010,7 @@
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B52" s="5"/>
       <c r="D52" s="5"/>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="12" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="B53" s="5"/>
       <c r="D53" s="5"/>
@@ -2055,7 +2058,7 @@
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="12" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B54" s="5"/>
       <c r="D54" s="5"/>
@@ -2074,12 +2077,12 @@
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
-      <c r="V54" s="5"/>
+      <c r="V54" s="1"/>
       <c r="W54" s="7"/>
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="12" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B55" s="5"/>
       <c r="D55" s="5"/>
@@ -2103,7 +2106,7 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B56" s="5"/>
       <c r="D56" s="5"/>
@@ -2127,7 +2130,7 @@
     </row>
     <row r="57" spans="1:23">
       <c r="A57" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B57" s="5"/>
       <c r="D57" s="5"/>
@@ -2151,7 +2154,7 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B58" s="5"/>
       <c r="D58" s="5"/>
@@ -2175,7 +2178,7 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59" s="5"/>
       <c r="D59" s="5"/>
@@ -2199,7 +2202,7 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="5"/>
       <c r="D60" s="5"/>
@@ -2222,8 +2225,8 @@
       <c r="W60" s="7"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="13" t="s">
-        <v>67</v>
+      <c r="A61" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="B61" s="5"/>
       <c r="D61" s="5"/>
@@ -2246,8 +2249,8 @@
       <c r="W61" s="7"/>
     </row>
     <row r="62" spans="1:23">
-      <c r="A62" s="12" t="s">
-        <v>49</v>
+      <c r="A62" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B62" s="5"/>
       <c r="D62" s="5"/>
@@ -2271,7 +2274,7 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="12" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B63" s="5"/>
       <c r="D63" s="5"/>
@@ -2295,7 +2298,7 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B64" s="5"/>
       <c r="D64" s="5"/>
@@ -2319,7 +2322,7 @@
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="12" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B65" s="5"/>
       <c r="D65" s="5"/>
@@ -2343,7 +2346,7 @@
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="12" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B66" s="5"/>
       <c r="D66" s="5"/>
@@ -2367,7 +2370,7 @@
     </row>
     <row r="67" spans="1:23">
       <c r="A67" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="5"/>
       <c r="D67" s="5"/>
@@ -2391,7 +2394,7 @@
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="12" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B68" s="5"/>
       <c r="D68" s="5"/>
@@ -2415,7 +2418,7 @@
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B69" s="5"/>
       <c r="D69" s="5"/>
@@ -2439,7 +2442,7 @@
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="12" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B70" s="5"/>
       <c r="D70" s="5"/>
@@ -2463,7 +2466,7 @@
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B71" s="5"/>
       <c r="D71" s="5"/>
@@ -2487,7 +2490,7 @@
     </row>
     <row r="72" spans="1:23">
       <c r="A72" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B72" s="5"/>
       <c r="D72" s="5"/>
@@ -2511,7 +2514,7 @@
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B73" s="5"/>
       <c r="D73" s="5"/>
@@ -2535,7 +2538,7 @@
     </row>
     <row r="74" spans="1:23">
       <c r="A74" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B74" s="5"/>
       <c r="D74" s="5"/>
@@ -2554,12 +2557,12 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5"/>
-      <c r="V74" s="1"/>
+      <c r="V74" s="5"/>
       <c r="W74" s="7"/>
     </row>
     <row r="75" spans="1:23">
       <c r="A75" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" s="5"/>
       <c r="D75" s="5"/>
@@ -2583,7 +2586,7 @@
     </row>
     <row r="76" spans="1:23">
       <c r="A76" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B76" s="5"/>
       <c r="D76" s="5"/>
@@ -2607,7 +2610,7 @@
     </row>
     <row r="77" spans="1:23">
       <c r="A77" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B77" s="5"/>
       <c r="D77" s="5"/>
@@ -2631,7 +2634,7 @@
     </row>
     <row r="78" spans="1:23">
       <c r="A78" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78" s="5"/>
       <c r="D78" s="5"/>
@@ -2650,12 +2653,12 @@
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
       <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
+      <c r="V78" s="1"/>
       <c r="W78" s="7"/>
     </row>
     <row r="79" spans="1:23">
       <c r="A79" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B79" s="5"/>
       <c r="D79" s="5"/>
@@ -2679,7 +2682,7 @@
     </row>
     <row r="80" spans="1:23">
       <c r="A80" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80" s="5"/>
       <c r="D80" s="5"/>
@@ -2698,12 +2701,12 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
-      <c r="V80" s="1"/>
+      <c r="V80" s="5"/>
       <c r="W80" s="7"/>
     </row>
     <row r="81" spans="1:23">
       <c r="A81" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B81" s="5"/>
       <c r="D81" s="5"/>
@@ -2727,7 +2730,7 @@
     </row>
     <row r="82" spans="1:23">
       <c r="A82" s="12" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B82" s="5"/>
       <c r="D82" s="5"/>
@@ -2751,7 +2754,7 @@
     </row>
     <row r="83" spans="1:23">
       <c r="A83" s="12" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B83" s="5"/>
       <c r="D83" s="5"/>
@@ -2775,7 +2778,7 @@
     </row>
     <row r="84" spans="1:23">
       <c r="A84" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B84" s="5"/>
       <c r="D84" s="5"/>
@@ -2799,7 +2802,7 @@
     </row>
     <row r="85" spans="1:23">
       <c r="A85" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="5"/>
       <c r="D85" s="5"/>
@@ -2818,12 +2821,12 @@
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
       <c r="U85" s="5"/>
-      <c r="V85" s="5"/>
+      <c r="V85" s="1"/>
       <c r="W85" s="7"/>
     </row>
     <row r="86" spans="1:23">
       <c r="A86" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B86" s="5"/>
       <c r="D86" s="5"/>
@@ -2847,7 +2850,7 @@
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B87" s="5"/>
       <c r="D87" s="5"/>
@@ -2871,7 +2874,7 @@
     </row>
     <row r="88" spans="1:23">
       <c r="A88" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B88" s="5"/>
       <c r="D88" s="5"/>
@@ -2895,7 +2898,7 @@
     </row>
     <row r="89" spans="1:23">
       <c r="A89" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" s="5"/>
       <c r="D89" s="5"/>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="90" spans="1:23">
       <c r="A90" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90" s="5"/>
       <c r="D90" s="5"/>
@@ -2943,7 +2946,7 @@
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B91" s="5"/>
       <c r="D91" s="5"/>
@@ -2967,7 +2970,7 @@
     </row>
     <row r="92" spans="1:23">
       <c r="A92" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B92" s="5"/>
       <c r="D92" s="5"/>
@@ -2991,7 +2994,7 @@
     </row>
     <row r="93" spans="1:23">
       <c r="A93" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" s="5"/>
       <c r="D93" s="5"/>
@@ -3015,7 +3018,7 @@
     </row>
     <row r="94" spans="1:23">
       <c r="A94" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" s="5"/>
       <c r="D94" s="5"/>
@@ -3039,7 +3042,7 @@
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="5"/>
       <c r="D95" s="5"/>
@@ -3063,10 +3066,9 @@
     </row>
     <row r="96" spans="1:23">
       <c r="A96" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="H96" s="5"/>
@@ -3088,7 +3090,7 @@
     </row>
     <row r="97" spans="1:23">
       <c r="A97" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
@@ -3113,7 +3115,7 @@
     </row>
     <row r="98" spans="1:23">
       <c r="A98" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -3138,7 +3140,7 @@
     </row>
     <row r="99" spans="1:23">
       <c r="A99" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -3163,7 +3165,7 @@
     </row>
     <row r="100" spans="1:23">
       <c r="A100" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -3188,7 +3190,7 @@
     </row>
     <row r="101" spans="1:23">
       <c r="A101" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
@@ -3208,12 +3210,12 @@
       <c r="S101" s="5"/>
       <c r="T101" s="5"/>
       <c r="U101" s="5"/>
-      <c r="V101" s="1"/>
+      <c r="V101" s="5"/>
       <c r="W101" s="7"/>
     </row>
     <row r="102" spans="1:23">
       <c r="A102" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
@@ -3237,7 +3239,9 @@
       <c r="W102" s="7"/>
     </row>
     <row r="103" spans="1:23">
-      <c r="A103" s="3"/>
+      <c r="A103" s="12" t="s">
+        <v>101</v>
+      </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -3256,7 +3260,7 @@
       <c r="S103" s="5"/>
       <c r="T103" s="5"/>
       <c r="U103" s="5"/>
-      <c r="V103" s="5"/>
+      <c r="V103" s="1"/>
       <c r="W103" s="7"/>
     </row>
     <row r="104" spans="1:23">
@@ -3394,7 +3398,7 @@
       <c r="S109" s="5"/>
       <c r="T109" s="5"/>
       <c r="U109" s="5"/>
-      <c r="V109" s="1"/>
+      <c r="V109" s="5"/>
       <c r="W109" s="7"/>
     </row>
     <row r="110" spans="1:23">
@@ -3421,6 +3425,7 @@
       <c r="W110" s="7"/>
     </row>
     <row r="111" spans="1:23">
+      <c r="A111" s="3"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -3439,7 +3444,7 @@
       <c r="S111" s="5"/>
       <c r="T111" s="5"/>
       <c r="U111" s="5"/>
-      <c r="V111" s="5"/>
+      <c r="V111" s="1"/>
       <c r="W111" s="7"/>
     </row>
     <row r="112" spans="1:23">
@@ -3615,7 +3620,7 @@
       <c r="S119" s="5"/>
       <c r="T119" s="5"/>
       <c r="U119" s="5"/>
-      <c r="V119" s="1"/>
+      <c r="V119" s="5"/>
       <c r="W119" s="7"/>
     </row>
     <row r="120" spans="1:23">
@@ -3707,7 +3712,6 @@
       <c r="W123" s="7"/>
     </row>
     <row r="124" spans="1:23">
-      <c r="A124" s="3"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -3730,6 +3734,7 @@
       <c r="W124" s="7"/>
     </row>
     <row r="125" spans="1:23">
+      <c r="A125" s="3"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -3836,7 +3841,7 @@
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
       <c r="U129" s="5"/>
-      <c r="V129" s="5"/>
+      <c r="V129" s="1"/>
       <c r="W129" s="7"/>
     </row>
     <row r="130" spans="1:23">
@@ -3862,7 +3867,6 @@
       <c r="W130" s="7"/>
     </row>
     <row r="131" spans="1:23">
-      <c r="A131" s="3"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -3881,10 +3885,11 @@
       <c r="S131" s="5"/>
       <c r="T131" s="5"/>
       <c r="U131" s="5"/>
-      <c r="V131" s="1"/>
+      <c r="V131" s="5"/>
       <c r="W131" s="7"/>
     </row>
     <row r="132" spans="1:23">
+      <c r="A132" s="3"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -3903,11 +3908,10 @@
       <c r="S132" s="5"/>
       <c r="T132" s="5"/>
       <c r="U132" s="5"/>
-      <c r="V132" s="5"/>
+      <c r="V132" s="1"/>
       <c r="W132" s="7"/>
     </row>
     <row r="133" spans="1:23">
-      <c r="A133" s="3"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -3930,6 +3934,7 @@
       <c r="W133" s="7"/>
     </row>
     <row r="134" spans="1:23">
+      <c r="A134" s="3"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -3948,7 +3953,7 @@
       <c r="S134" s="5"/>
       <c r="T134" s="5"/>
       <c r="U134" s="5"/>
-      <c r="V134" s="1"/>
+      <c r="V134" s="5"/>
       <c r="W134" s="7"/>
     </row>
     <row r="135" spans="1:23">
@@ -4146,7 +4151,7 @@
       <c r="S143" s="5"/>
       <c r="T143" s="5"/>
       <c r="U143" s="5"/>
-      <c r="V143" s="5"/>
+      <c r="V143" s="1"/>
       <c r="W143" s="7"/>
     </row>
     <row r="144" spans="1:23">
@@ -4190,7 +4195,7 @@
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
       <c r="U145" s="5"/>
-      <c r="V145" s="1"/>
+      <c r="V145" s="5"/>
       <c r="W145" s="7"/>
     </row>
     <row r="146" spans="2:23">
@@ -4212,7 +4217,7 @@
       <c r="S146" s="5"/>
       <c r="T146" s="5"/>
       <c r="U146" s="5"/>
-      <c r="V146" s="5"/>
+      <c r="V146" s="1"/>
       <c r="W146" s="7"/>
     </row>
     <row r="147" spans="2:23">
@@ -4278,7 +4283,7 @@
       <c r="S149" s="5"/>
       <c r="T149" s="5"/>
       <c r="U149" s="5"/>
-      <c r="V149" s="1"/>
+      <c r="V149" s="5"/>
       <c r="W149" s="7"/>
     </row>
     <row r="150" spans="2:23">
@@ -4322,7 +4327,7 @@
       <c r="S151" s="5"/>
       <c r="T151" s="5"/>
       <c r="U151" s="5"/>
-      <c r="V151" s="5"/>
+      <c r="V151" s="1"/>
       <c r="W151" s="7"/>
     </row>
     <row r="152" spans="2:23">
@@ -4674,7 +4679,7 @@
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
       <c r="U167" s="5"/>
-      <c r="V167" s="1"/>
+      <c r="V167" s="5"/>
       <c r="W167" s="7"/>
     </row>
     <row r="168" spans="2:23">
@@ -4718,7 +4723,7 @@
       <c r="S169" s="5"/>
       <c r="T169" s="5"/>
       <c r="U169" s="5"/>
-      <c r="V169" s="5"/>
+      <c r="V169" s="1"/>
       <c r="W169" s="7"/>
     </row>
     <row r="170" spans="2:23">
@@ -4762,7 +4767,7 @@
       <c r="S171" s="5"/>
       <c r="T171" s="5"/>
       <c r="U171" s="5"/>
-      <c r="V171" s="1"/>
+      <c r="V171" s="5"/>
       <c r="W171" s="7"/>
     </row>
     <row r="172" spans="2:23">
@@ -4806,7 +4811,7 @@
       <c r="S173" s="5"/>
       <c r="T173" s="5"/>
       <c r="U173" s="5"/>
-      <c r="V173" s="5"/>
+      <c r="V173" s="1"/>
       <c r="W173" s="7"/>
     </row>
     <row r="174" spans="2:23">
@@ -5158,7 +5163,7 @@
       <c r="S189" s="5"/>
       <c r="T189" s="5"/>
       <c r="U189" s="5"/>
-      <c r="V189" s="1"/>
+      <c r="V189" s="5"/>
       <c r="W189" s="7"/>
     </row>
     <row r="190" spans="2:23">
@@ -5246,7 +5251,7 @@
       <c r="S193" s="5"/>
       <c r="T193" s="5"/>
       <c r="U193" s="5"/>
-      <c r="V193" s="5"/>
+      <c r="V193" s="1"/>
       <c r="W193" s="7"/>
     </row>
     <row r="194" spans="2:23">
@@ -5334,7 +5339,7 @@
       <c r="S197" s="5"/>
       <c r="T197" s="5"/>
       <c r="U197" s="5"/>
-      <c r="V197" s="1"/>
+      <c r="V197" s="5"/>
       <c r="W197" s="7"/>
     </row>
     <row r="198" spans="2:23">
@@ -5378,7 +5383,7 @@
       <c r="S199" s="5"/>
       <c r="T199" s="5"/>
       <c r="U199" s="5"/>
-      <c r="V199" s="5"/>
+      <c r="V199" s="1"/>
       <c r="W199" s="7"/>
     </row>
     <row r="200" spans="2:23">
@@ -5598,7 +5603,7 @@
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
-      <c r="V209" s="1"/>
+      <c r="V209" s="5"/>
       <c r="W209" s="7"/>
     </row>
     <row r="210" spans="1:23">
@@ -5624,7 +5629,6 @@
       <c r="W210" s="7"/>
     </row>
     <row r="211" spans="1:23">
-      <c r="A211" s="3"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
@@ -5643,10 +5647,11 @@
       <c r="S211" s="5"/>
       <c r="T211" s="5"/>
       <c r="U211" s="5"/>
-      <c r="V211" s="5"/>
+      <c r="V211" s="1"/>
       <c r="W211" s="7"/>
     </row>
     <row r="212" spans="1:23">
+      <c r="A212" s="3"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
@@ -5669,7 +5674,6 @@
       <c r="W212" s="7"/>
     </row>
     <row r="213" spans="1:23">
-      <c r="A213" s="8"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
@@ -5692,7 +5696,7 @@
       <c r="W213" s="7"/>
     </row>
     <row r="214" spans="1:23">
-      <c r="A214" s="3"/>
+      <c r="A214" s="8"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
@@ -5734,10 +5738,11 @@
       <c r="S215" s="5"/>
       <c r="T215" s="5"/>
       <c r="U215" s="5"/>
-      <c r="V215" s="1"/>
+      <c r="V215" s="5"/>
       <c r="W215" s="7"/>
     </row>
     <row r="216" spans="1:23">
+      <c r="A216" s="3"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
@@ -5778,7 +5783,7 @@
       <c r="S217" s="5"/>
       <c r="T217" s="5"/>
       <c r="U217" s="5"/>
-      <c r="V217" s="5"/>
+      <c r="V217" s="1"/>
       <c r="W217" s="7"/>
     </row>
     <row r="218" spans="1:23">
@@ -6222,7 +6227,6 @@
       <c r="W237" s="7"/>
     </row>
     <row r="238" spans="1:23">
-      <c r="A238" s="8"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
       <c r="D238" s="5"/>
@@ -6245,6 +6249,7 @@
       <c r="W238" s="7"/>
     </row>
     <row r="239" spans="1:23">
+      <c r="A239" s="8"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
       <c r="D239" s="5"/>
@@ -6267,7 +6272,6 @@
       <c r="W239" s="7"/>
     </row>
     <row r="240" spans="1:23">
-      <c r="A240" s="8"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
       <c r="D240" s="5"/>
@@ -6290,7 +6294,7 @@
       <c r="W240" s="7"/>
     </row>
     <row r="241" spans="1:23">
-      <c r="A241" s="3"/>
+      <c r="A241" s="8"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
       <c r="D241" s="5"/>
@@ -6313,6 +6317,7 @@
       <c r="W241" s="7"/>
     </row>
     <row r="242" spans="1:23">
+      <c r="A242" s="3"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
       <c r="D242" s="5"/>
@@ -6353,7 +6358,7 @@
       <c r="S243" s="5"/>
       <c r="T243" s="5"/>
       <c r="U243" s="5"/>
-      <c r="V243" s="1"/>
+      <c r="V243" s="5"/>
       <c r="W243" s="7"/>
     </row>
     <row r="244" spans="1:23">
@@ -6379,7 +6384,6 @@
       <c r="W244" s="7"/>
     </row>
     <row r="245" spans="1:23">
-      <c r="A245" s="8"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
       <c r="D245" s="5"/>
@@ -6398,10 +6402,11 @@
       <c r="S245" s="5"/>
       <c r="T245" s="5"/>
       <c r="U245" s="5"/>
-      <c r="V245" s="5"/>
+      <c r="V245" s="1"/>
       <c r="W245" s="7"/>
     </row>
     <row r="246" spans="1:23">
+      <c r="A246" s="8"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
       <c r="D246" s="5"/>
@@ -6424,7 +6429,6 @@
       <c r="W246" s="7"/>
     </row>
     <row r="247" spans="1:23">
-      <c r="A247" s="8"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
       <c r="D247" s="5"/>
@@ -6443,10 +6447,11 @@
       <c r="S247" s="5"/>
       <c r="T247" s="5"/>
       <c r="U247" s="5"/>
-      <c r="V247" s="1"/>
+      <c r="V247" s="5"/>
       <c r="W247" s="7"/>
     </row>
     <row r="248" spans="1:23">
+      <c r="A248" s="8"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
       <c r="D248" s="5"/>
@@ -6465,7 +6470,7 @@
       <c r="S248" s="5"/>
       <c r="T248" s="5"/>
       <c r="U248" s="5"/>
-      <c r="V248" s="5"/>
+      <c r="V248" s="1"/>
       <c r="W248" s="7"/>
     </row>
     <row r="249" spans="1:23">
@@ -6509,7 +6514,7 @@
       <c r="S250" s="5"/>
       <c r="T250" s="5"/>
       <c r="U250" s="5"/>
-      <c r="V250" s="1"/>
+      <c r="V250" s="5"/>
       <c r="W250" s="7"/>
     </row>
     <row r="251" spans="1:23">
@@ -6597,7 +6602,7 @@
       <c r="S254" s="5"/>
       <c r="T254" s="5"/>
       <c r="U254" s="5"/>
-      <c r="V254" s="5"/>
+      <c r="V254" s="1"/>
       <c r="W254" s="7"/>
     </row>
     <row r="255" spans="1:23">
@@ -6685,7 +6690,7 @@
       <c r="S258" s="5"/>
       <c r="T258" s="5"/>
       <c r="U258" s="5"/>
-      <c r="V258" s="1"/>
+      <c r="V258" s="5"/>
       <c r="W258" s="7"/>
     </row>
     <row r="259" spans="2:23">
@@ -6729,7 +6734,7 @@
       <c r="S260" s="5"/>
       <c r="T260" s="5"/>
       <c r="U260" s="5"/>
-      <c r="V260" s="5"/>
+      <c r="V260" s="1"/>
       <c r="W260" s="7"/>
     </row>
     <row r="261" spans="2:23">
@@ -7301,7 +7306,7 @@
       <c r="S286" s="5"/>
       <c r="T286" s="5"/>
       <c r="U286" s="5"/>
-      <c r="V286" s="1"/>
+      <c r="V286" s="5"/>
       <c r="W286" s="7"/>
     </row>
     <row r="287" spans="2:23">
@@ -7345,7 +7350,7 @@
       <c r="S288" s="5"/>
       <c r="T288" s="5"/>
       <c r="U288" s="5"/>
-      <c r="V288" s="5"/>
+      <c r="V288" s="1"/>
       <c r="W288" s="7"/>
     </row>
     <row r="289" spans="2:23">
@@ -7389,7 +7394,7 @@
       <c r="S290" s="5"/>
       <c r="T290" s="5"/>
       <c r="U290" s="5"/>
-      <c r="V290" s="1"/>
+      <c r="V290" s="5"/>
       <c r="W290" s="7"/>
     </row>
     <row r="291" spans="2:23">
@@ -7411,7 +7416,7 @@
       <c r="S291" s="5"/>
       <c r="T291" s="5"/>
       <c r="U291" s="5"/>
-      <c r="V291" s="5"/>
+      <c r="V291" s="1"/>
       <c r="W291" s="7"/>
     </row>
     <row r="292" spans="2:23">
@@ -7961,7 +7966,7 @@
       <c r="S316" s="5"/>
       <c r="T316" s="5"/>
       <c r="U316" s="5"/>
-      <c r="V316" s="1"/>
+      <c r="V316" s="5"/>
       <c r="W316" s="7"/>
     </row>
     <row r="317" spans="2:23">
@@ -8071,7 +8076,7 @@
       <c r="S321" s="5"/>
       <c r="T321" s="5"/>
       <c r="U321" s="5"/>
-      <c r="V321" s="5"/>
+      <c r="V321" s="1"/>
       <c r="W321" s="7"/>
     </row>
     <row r="322" spans="2:23">
@@ -8159,7 +8164,7 @@
       <c r="S325" s="5"/>
       <c r="T325" s="5"/>
       <c r="U325" s="5"/>
-      <c r="V325" s="1"/>
+      <c r="V325" s="5"/>
       <c r="W325" s="7"/>
     </row>
     <row r="326" spans="2:23">
@@ -8203,7 +8208,7 @@
       <c r="S327" s="5"/>
       <c r="T327" s="5"/>
       <c r="U327" s="5"/>
-      <c r="V327" s="5"/>
+      <c r="V327" s="1"/>
       <c r="W327" s="7"/>
     </row>
     <row r="328" spans="2:23">
@@ -8247,7 +8252,7 @@
       <c r="S329" s="5"/>
       <c r="T329" s="5"/>
       <c r="U329" s="5"/>
-      <c r="V329" s="1"/>
+      <c r="V329" s="5"/>
       <c r="W329" s="7"/>
     </row>
     <row r="330" spans="2:23">
@@ -8291,7 +8296,7 @@
       <c r="S331" s="5"/>
       <c r="T331" s="5"/>
       <c r="U331" s="5"/>
-      <c r="V331" s="5"/>
+      <c r="V331" s="1"/>
       <c r="W331" s="7"/>
     </row>
     <row r="332" spans="2:23">
@@ -8643,7 +8648,7 @@
       <c r="S347" s="5"/>
       <c r="T347" s="5"/>
       <c r="U347" s="5"/>
-      <c r="V347" s="1"/>
+      <c r="V347" s="5"/>
       <c r="W347" s="7"/>
     </row>
     <row r="348" spans="2:23">
@@ -8687,7 +8692,7 @@
       <c r="S349" s="5"/>
       <c r="T349" s="5"/>
       <c r="U349" s="5"/>
-      <c r="V349" s="5"/>
+      <c r="V349" s="1"/>
       <c r="W349" s="7"/>
     </row>
     <row r="350" spans="2:23">
@@ -8819,7 +8824,7 @@
       <c r="S355" s="5"/>
       <c r="T355" s="5"/>
       <c r="U355" s="5"/>
-      <c r="V355" s="1"/>
+      <c r="V355" s="5"/>
       <c r="W355" s="7"/>
     </row>
     <row r="356" spans="2:23">
@@ -8863,7 +8868,7 @@
       <c r="S357" s="5"/>
       <c r="T357" s="5"/>
       <c r="U357" s="5"/>
-      <c r="V357" s="5"/>
+      <c r="V357" s="1"/>
       <c r="W357" s="7"/>
     </row>
     <row r="358" spans="2:23">
@@ -8907,7 +8912,7 @@
       <c r="S359" s="5"/>
       <c r="T359" s="5"/>
       <c r="U359" s="5"/>
-      <c r="V359" s="1"/>
+      <c r="V359" s="5"/>
       <c r="W359" s="7"/>
     </row>
     <row r="360" spans="2:23">
@@ -8929,7 +8934,7 @@
       <c r="S360" s="5"/>
       <c r="T360" s="5"/>
       <c r="U360" s="5"/>
-      <c r="V360" s="5"/>
+      <c r="V360" s="1"/>
       <c r="W360" s="7"/>
     </row>
     <row r="361" spans="2:23">
@@ -9391,7 +9396,7 @@
       <c r="S381" s="5"/>
       <c r="T381" s="5"/>
       <c r="U381" s="5"/>
-      <c r="V381" s="1"/>
+      <c r="V381" s="5"/>
       <c r="W381" s="7"/>
     </row>
     <row r="382" spans="2:23">
@@ -9501,7 +9506,7 @@
       <c r="S386" s="5"/>
       <c r="T386" s="5"/>
       <c r="U386" s="5"/>
-      <c r="V386" s="5"/>
+      <c r="V386" s="1"/>
       <c r="W386" s="7"/>
     </row>
     <row r="387" spans="2:23">
@@ -9589,7 +9594,7 @@
       <c r="S390" s="5"/>
       <c r="T390" s="5"/>
       <c r="U390" s="5"/>
-      <c r="V390" s="1"/>
+      <c r="V390" s="5"/>
       <c r="W390" s="7"/>
     </row>
     <row r="391" spans="2:23">
@@ -9633,7 +9638,7 @@
       <c r="S392" s="5"/>
       <c r="T392" s="5"/>
       <c r="U392" s="5"/>
-      <c r="V392" s="5"/>
+      <c r="V392" s="1"/>
       <c r="W392" s="7"/>
     </row>
     <row r="393" spans="2:23">
@@ -9677,7 +9682,7 @@
       <c r="S394" s="5"/>
       <c r="T394" s="5"/>
       <c r="U394" s="5"/>
-      <c r="V394" s="1"/>
+      <c r="V394" s="5"/>
       <c r="W394" s="7"/>
     </row>
     <row r="395" spans="2:23">
@@ -9721,7 +9726,7 @@
       <c r="S396" s="5"/>
       <c r="T396" s="5"/>
       <c r="U396" s="5"/>
-      <c r="V396" s="5"/>
+      <c r="V396" s="1"/>
       <c r="W396" s="7"/>
     </row>
     <row r="397" spans="2:23">
@@ -9989,7 +9994,6 @@
       <c r="W408" s="7"/>
     </row>
     <row r="409" spans="1:23">
-      <c r="A409" s="8"/>
       <c r="B409" s="5"/>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -10012,6 +10016,7 @@
       <c r="W409" s="7"/>
     </row>
     <row r="410" spans="1:23">
+      <c r="A410" s="8"/>
       <c r="B410" s="5"/>
       <c r="C410" s="5"/>
       <c r="D410" s="5"/>
@@ -10074,7 +10079,7 @@
       <c r="S412" s="5"/>
       <c r="T412" s="5"/>
       <c r="U412" s="5"/>
-      <c r="V412" s="1"/>
+      <c r="V412" s="5"/>
       <c r="W412" s="7"/>
     </row>
     <row r="413" spans="1:23">
@@ -10118,7 +10123,7 @@
       <c r="S414" s="5"/>
       <c r="T414" s="5"/>
       <c r="U414" s="5"/>
-      <c r="V414" s="5"/>
+      <c r="V414" s="1"/>
       <c r="W414" s="7"/>
     </row>
     <row r="415" spans="1:23">
@@ -10144,7 +10149,6 @@
       <c r="W415" s="7"/>
     </row>
     <row r="416" spans="1:23">
-      <c r="A416" s="3"/>
       <c r="B416" s="5"/>
       <c r="C416" s="5"/>
       <c r="D416" s="5"/>
@@ -10167,7 +10171,7 @@
       <c r="W416" s="7"/>
     </row>
     <row r="417" spans="1:23">
-      <c r="A417" s="8"/>
+      <c r="A417" s="3"/>
       <c r="B417" s="5"/>
       <c r="C417" s="5"/>
       <c r="D417" s="5"/>
@@ -10190,6 +10194,7 @@
       <c r="W417" s="7"/>
     </row>
     <row r="418" spans="1:23">
+      <c r="A418" s="8"/>
       <c r="B418" s="5"/>
       <c r="C418" s="5"/>
       <c r="D418" s="5"/>
@@ -10252,7 +10257,7 @@
       <c r="S420" s="5"/>
       <c r="T420" s="5"/>
       <c r="U420" s="5"/>
-      <c r="V420" s="1"/>
+      <c r="V420" s="5"/>
       <c r="W420" s="7"/>
     </row>
     <row r="421" spans="1:23">
@@ -10296,7 +10301,7 @@
       <c r="S422" s="5"/>
       <c r="T422" s="5"/>
       <c r="U422" s="5"/>
-      <c r="V422" s="5"/>
+      <c r="V422" s="1"/>
       <c r="W422" s="7"/>
     </row>
     <row r="423" spans="1:23">
@@ -10340,8 +10345,30 @@
       <c r="S424" s="5"/>
       <c r="T424" s="5"/>
       <c r="U424" s="5"/>
-      <c r="V424" s="1"/>
+      <c r="V424" s="5"/>
       <c r="W424" s="7"/>
+    </row>
+    <row r="425" spans="1:23">
+      <c r="B425" s="5"/>
+      <c r="C425" s="5"/>
+      <c r="D425" s="5"/>
+      <c r="E425" s="5"/>
+      <c r="H425" s="5"/>
+      <c r="I425" s="5"/>
+      <c r="J425" s="5"/>
+      <c r="K425" s="5"/>
+      <c r="L425" s="5"/>
+      <c r="M425" s="6"/>
+      <c r="N425" s="5"/>
+      <c r="O425" s="5"/>
+      <c r="P425" s="5"/>
+      <c r="Q425" s="5"/>
+      <c r="R425" s="5"/>
+      <c r="S425" s="5"/>
+      <c r="T425" s="5"/>
+      <c r="U425" s="5"/>
+      <c r="V425" s="1"/>
+      <c r="W425" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>